<commit_message>
Update documents for evidence
</commit_message>
<xml_diff>
--- a/Resources/01_mega_movie_fundraiser.xlsx
+++ b/Resources/01_mega_movie_fundraiser.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20367"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://masseyhighschoolnz-my.sharepoint.com/personal/jgottschalk_masseyhigh_school_nz/Documents/Projects/01_Tutorials/12I_91896_7_v2_Adv_Programming_Revisited/91896_7_v2_support_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aroof\Documents\Programming\L2_MMF\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="8_{9380B24E-17DF-453D-8434-8CC8ACE91486}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{02877C51-2392-44C6-A06E-55B200A53712}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{240D9900-0308-47AC-8458-C65BADDFF91B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{31E039A0-BFD1-4590-9D50-EC525F3332F7}"/>
   </bookViews>
@@ -20,15 +20,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -800,10 +791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41873174-3C06-4FAD-B97F-02F649204032}">
-  <dimension ref="A1:P13"/>
+  <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I9"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,12 +898,12 @@
         <v>2.5</v>
       </c>
       <c r="O2" s="2">
-        <f>L2*0.2</f>
-        <v>3.3000000000000003</v>
+        <f>I2*0.2</f>
+        <v>1.8</v>
       </c>
       <c r="P2" s="2">
         <f>N2+O2</f>
-        <v>5.8000000000000007</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -952,12 +943,12 @@
         <v>5.5</v>
       </c>
       <c r="O3" s="2">
-        <f t="shared" ref="O3:O10" si="5">L3*0.2</f>
-        <v>3.1</v>
+        <f t="shared" ref="O3:O10" si="5">I3*0.2</f>
+        <v>1</v>
       </c>
       <c r="P3" s="2">
         <f t="shared" ref="P3:P10" si="6">N3+O3</f>
-        <v>8.6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -995,11 +986,11 @@
       </c>
       <c r="O4" s="2">
         <f t="shared" si="5"/>
-        <v>2.8875000000000002</v>
+        <v>0.65</v>
       </c>
       <c r="P4" s="2">
         <f t="shared" si="6"/>
-        <v>8.3874999999999993</v>
+        <v>6.15</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1040,11 +1031,11 @@
       </c>
       <c r="O5" s="2">
         <f t="shared" si="5"/>
-        <v>3.1500000000000004</v>
+        <v>0.9</v>
       </c>
       <c r="P5" s="2">
         <f t="shared" si="6"/>
-        <v>8.65</v>
+        <v>6.4</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1064,12 +1055,9 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
       <c r="I6" s="2">
         <f t="shared" si="1"/>
-        <v>9.5</v>
+        <v>7.5</v>
       </c>
       <c r="J6" t="s">
         <v>29</v>
@@ -1080,7 +1068,7 @@
       </c>
       <c r="L6" s="2">
         <f t="shared" si="3"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="N6" s="2">
         <f t="shared" si="4"/>
@@ -1088,11 +1076,11 @@
       </c>
       <c r="O6" s="2">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>1.5</v>
       </c>
       <c r="P6" s="2">
         <f t="shared" si="6"/>
-        <v>9.5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1133,11 +1121,11 @@
       </c>
       <c r="O7" s="2">
         <f t="shared" si="5"/>
-        <v>2.4500000000000002</v>
+        <v>1.1500000000000001</v>
       </c>
       <c r="P7" s="2">
         <f t="shared" si="6"/>
-        <v>3.95</v>
+        <v>2.6500000000000004</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1178,11 +1166,11 @@
       </c>
       <c r="O8" s="2">
         <f t="shared" si="5"/>
-        <v>3.8325000000000005</v>
+        <v>1.55</v>
       </c>
       <c r="P8" s="2">
         <f t="shared" si="6"/>
-        <v>9.3324999999999996</v>
+        <v>7.05</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1223,11 +1211,11 @@
       </c>
       <c r="O9" s="2">
         <f t="shared" si="5"/>
-        <v>3.1</v>
+        <v>1</v>
       </c>
       <c r="P9" s="2">
         <f t="shared" si="6"/>
-        <v>8.6</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1268,11 +1256,11 @@
       </c>
       <c r="O10" s="2">
         <f t="shared" si="5"/>
-        <v>3.25</v>
+        <v>1.1500000000000001</v>
       </c>
       <c r="P10" s="2">
         <f t="shared" si="6"/>
-        <v>8.75</v>
+        <v>6.65</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
@@ -1297,7 +1285,7 @@
       </c>
       <c r="H12">
         <f t="shared" si="7"/>
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
@@ -1313,8 +1301,11 @@
       </c>
       <c r="P13" s="10">
         <f>SUM(P2:P12)</f>
-        <v>71.569999999999993</v>
-      </c>
+        <v>53.199999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>